<commit_message>
changed by Sam's request
</commit_message>
<xml_diff>
--- a/Documents/pin definition.xlsx
+++ b/Documents/pin definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A50807\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Side Project\AgileSwitch-dsPIC33CK\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7886BCA9-1325-420F-ADF8-AD5B2AAADD5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41510E96-EA44-4535-A972-0AA54879BF16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="1815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pin definition" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>50K / 100K Hz PWM signals for Hi Drive In+</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -128,6 +128,30 @@
   </si>
   <si>
     <t>LED3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperature decode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voltage decode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RP66_RD2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RP69_RD5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset Output</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RP72_RD8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -517,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +658,30 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>